<commit_message>
criado migration de colunas, para recerber novos dados e melhorar o sistema, tela de home listando imagem e dados, execel listado os dados e somando e baixando os dados corretamente
</commit_message>
<xml_diff>
--- a/public/template/lista.xlsx
+++ b/public/template/lista.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\visumOs\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E81B71D-42A8-45A6-A5CA-64FF867089B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6735AB-5647-4FD3-AF85-920AF7560049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{2C302A75-16A8-4378-A928-C1553DDDA203}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>PLANILHA DE MEDIÇÃO DE SERVIÇOS</t>
   </si>
@@ -62,34 +62,19 @@
     <t>Período:</t>
   </si>
   <si>
-    <t>20/11/24 a 15/12/24</t>
-  </si>
-  <si>
     <t>Data:</t>
   </si>
   <si>
     <t>Cidade:</t>
   </si>
   <si>
-    <t>Campinas</t>
-  </si>
-  <si>
     <t>Site:</t>
-  </si>
-  <si>
-    <t>SP1520W (HUB RONDON)</t>
   </si>
   <si>
     <t>Área Técnica:</t>
   </si>
   <si>
-    <t>CATAB</t>
-  </si>
-  <si>
     <t>Área/Node:</t>
-  </si>
-  <si>
-    <t>CATAB/PVIAE</t>
   </si>
   <si>
     <t>Código</t>
@@ -682,43 +667,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -726,85 +681,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="2" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="12" fontId="2" fillId="2" borderId="18" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -828,15 +714,6 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -848,15 +725,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -869,21 +737,6 @@
     </xf>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -898,33 +751,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="13" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -944,14 +770,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
@@ -962,12 +788,172 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="22" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="23" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="13" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="2" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="12" fontId="2" fillId="2" borderId="18" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -1280,11 +1266,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>314011</xdr:colOff>
+      <xdr:colOff>551576</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>167651</xdr:rowOff>
+      <xdr:rowOff>81538</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2784865" cy="781240"/>
+    <xdr:ext cx="2309735" cy="953466"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="6" name="CaixaDeTexto 5">
@@ -1298,8 +1284,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8515036" y="7863851"/>
-          <a:ext cx="2784865" cy="781240"/>
+          <a:off x="4818776" y="7501513"/>
+          <a:ext cx="2309735" cy="953466"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1368,19 +1354,46 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Data:     /     /</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="pt-BR" sz="1100" b="1"/>
-            <a:t>Data: </a:t>
+            <a:rPr lang="pt-BR" sz="1100" b="1" baseline="0"/>
+            <a:t> </a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100" b="1" baseline="0"/>
-            <a:t>     20 </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1100" b="1"/>
-            <a:t>/ 02 / 2024</a:t>
-          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1100" b="1"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1706,10 +1719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B25EF2AA-BC79-42C1-8634-CA5B31B1005A}">
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:K7"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1718,669 +1731,660 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="4" t="s">
+      <c r="A1" s="78"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="6"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="83"/>
+      <c r="K1" s="84"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="9" t="s">
+      <c r="A2" s="80"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="12"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="86"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="16"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="87"/>
+      <c r="K3" s="88"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="91">
         <v>5700013731</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="20"/>
+      <c r="C4" s="92"/>
+      <c r="D4" s="92"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="92"/>
+      <c r="H4" s="92"/>
+      <c r="I4" s="92"/>
+      <c r="J4" s="92"/>
+      <c r="K4" s="93"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="24"/>
+      <c r="C5" s="95"/>
+      <c r="D5" s="95"/>
+      <c r="E5" s="95"/>
+      <c r="F5" s="95"/>
+      <c r="G5" s="95"/>
+      <c r="H5" s="95"/>
+      <c r="I5" s="95"/>
+      <c r="J5" s="95"/>
+      <c r="K5" s="96"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="28"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="71"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="31"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="73"/>
+      <c r="H7" s="73"/>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="74"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="60"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="61"/>
+      <c r="I8" s="61"/>
+      <c r="J8" s="61"/>
+      <c r="K8" s="62"/>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="34"/>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="25" t="s">
+      <c r="B9" s="69"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="70"/>
+      <c r="H9" s="70"/>
+      <c r="I9" s="70"/>
+      <c r="J9" s="70"/>
+      <c r="K9" s="71"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="26">
-        <v>45641</v>
-      </c>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="28"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+      <c r="B10" s="75"/>
+      <c r="C10" s="76"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="76"/>
+      <c r="J10" s="76"/>
+      <c r="K10" s="77"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B11" s="60"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="61"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="61"/>
+      <c r="I11" s="61"/>
+      <c r="J11" s="61"/>
+      <c r="K11" s="62"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="36"/>
-      <c r="K10" s="37"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
+      <c r="B12" s="60"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="61"/>
+      <c r="J12" s="61"/>
+      <c r="K12" s="62"/>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B13" s="63"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="64"/>
+      <c r="I13" s="64"/>
+      <c r="J13" s="64"/>
+      <c r="K13" s="65"/>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="14"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="34"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
+      <c r="B15" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="C15" s="67"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="68"/>
+      <c r="H15" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="33"/>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="34"/>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="25" t="s">
+      <c r="I15" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="J15" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="41"/>
-    </row>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="42"/>
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="46"/>
-      <c r="K14" s="47"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="48" t="s">
+      <c r="K15" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="49" t="s">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="19"/>
+      <c r="B16" s="55"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="57"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="23"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="19"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="57"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="23"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="19"/>
+      <c r="B18" s="55"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="57"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="23"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="19"/>
+      <c r="B19" s="55"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="23"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="19"/>
+      <c r="B20" s="55"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="56"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="23"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="19"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="57"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="23"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="19"/>
+      <c r="B22" s="55"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="56"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="56"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="23"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="19"/>
+      <c r="B23" s="55"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="56"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="23"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="19"/>
+      <c r="B24" s="55"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="56"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="23"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="19"/>
+      <c r="B25" s="55"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+      <c r="G25" s="57"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="23"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="19"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="23"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="19"/>
+      <c r="B27" s="55"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="56"/>
+      <c r="G27" s="57"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="22"/>
+      <c r="K27" s="23"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="19"/>
+      <c r="B28" s="55"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="57"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="23"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="19"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="57"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="22"/>
+      <c r="K29" s="23"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="58" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="50"/>
-      <c r="D15" s="50"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="52" t="s">
+      <c r="B30" s="59"/>
+      <c r="C30" s="44">
+        <v>0</v>
+      </c>
+      <c r="D30" s="45"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="26">
+        <v>0</v>
+      </c>
+      <c r="J30" s="27"/>
+      <c r="K30" s="28"/>
+    </row>
+    <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="I15" s="53" t="s">
+      <c r="B31" s="43"/>
+      <c r="C31" s="44">
+        <v>0</v>
+      </c>
+      <c r="D31" s="45"/>
+      <c r="E31" s="46"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="26">
+        <v>0</v>
+      </c>
+      <c r="J31" s="27"/>
+      <c r="K31" s="28"/>
+    </row>
+    <row r="32" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="J15" s="52" t="s">
+      <c r="B32" s="48"/>
+      <c r="C32" s="49">
+        <v>0</v>
+      </c>
+      <c r="D32" s="50"/>
+      <c r="E32" s="51"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="26">
+        <v>0</v>
+      </c>
+      <c r="J32" s="27"/>
+      <c r="K32" s="28"/>
+    </row>
+    <row r="33" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="52"/>
+      <c r="B33" s="53"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="53"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="32">
+        <v>0</v>
+      </c>
+      <c r="J33" s="33"/>
+      <c r="K33" s="34"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="K15" s="54" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="55"/>
-      <c r="B16" s="56"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="57"/>
-      <c r="G16" s="58"/>
-      <c r="H16" s="59"/>
-      <c r="I16" s="60"/>
-      <c r="J16" s="61"/>
-      <c r="K16" s="62"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="55"/>
-      <c r="B17" s="56"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="58"/>
-      <c r="H17" s="59"/>
-      <c r="I17" s="60"/>
-      <c r="J17" s="61"/>
-      <c r="K17" s="62"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="55"/>
-      <c r="B18" s="56"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="58"/>
-      <c r="H18" s="59"/>
-      <c r="I18" s="60"/>
-      <c r="J18" s="61"/>
-      <c r="K18" s="62"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="55"/>
-      <c r="B19" s="56"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="57"/>
-      <c r="G19" s="58"/>
-      <c r="H19" s="59"/>
-      <c r="I19" s="60"/>
-      <c r="J19" s="61"/>
-      <c r="K19" s="62"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="55"/>
-      <c r="B20" s="56"/>
-      <c r="C20" s="57"/>
-      <c r="D20" s="57"/>
-      <c r="E20" s="57"/>
-      <c r="F20" s="57"/>
-      <c r="G20" s="58"/>
-      <c r="H20" s="59"/>
-      <c r="I20" s="60"/>
-      <c r="J20" s="61"/>
-      <c r="K20" s="62"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="55"/>
-      <c r="B21" s="56"/>
-      <c r="C21" s="57"/>
-      <c r="D21" s="57"/>
-      <c r="E21" s="57"/>
-      <c r="F21" s="57"/>
-      <c r="G21" s="58"/>
-      <c r="H21" s="59"/>
-      <c r="I21" s="60"/>
-      <c r="J21" s="61"/>
-      <c r="K21" s="62"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="55"/>
-      <c r="B22" s="56"/>
-      <c r="C22" s="57"/>
-      <c r="D22" s="57"/>
-      <c r="E22" s="57"/>
-      <c r="F22" s="57"/>
-      <c r="G22" s="58"/>
-      <c r="H22" s="59"/>
-      <c r="I22" s="60"/>
-      <c r="J22" s="61"/>
-      <c r="K22" s="62"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="55"/>
-      <c r="B23" s="56"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="57"/>
-      <c r="G23" s="58"/>
-      <c r="H23" s="59"/>
-      <c r="I23" s="60"/>
-      <c r="J23" s="61"/>
-      <c r="K23" s="62"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="55"/>
-      <c r="B24" s="56"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="57"/>
-      <c r="F24" s="57"/>
-      <c r="G24" s="58"/>
-      <c r="H24" s="59"/>
-      <c r="I24" s="60"/>
-      <c r="J24" s="61"/>
-      <c r="K24" s="62"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="55"/>
-      <c r="B25" s="56"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="58"/>
-      <c r="H25" s="59"/>
-      <c r="I25" s="60"/>
-      <c r="J25" s="61"/>
-      <c r="K25" s="62"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="55"/>
-      <c r="B26" s="56"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="57"/>
-      <c r="G26" s="58"/>
-      <c r="H26" s="59"/>
-      <c r="I26" s="60"/>
-      <c r="J26" s="61"/>
-      <c r="K26" s="62"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="55"/>
-      <c r="B27" s="56"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="57"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="59"/>
-      <c r="I27" s="60"/>
-      <c r="J27" s="61"/>
-      <c r="K27" s="62"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="55"/>
-      <c r="B28" s="56"/>
-      <c r="C28" s="57"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="57"/>
-      <c r="G28" s="58"/>
-      <c r="H28" s="59"/>
-      <c r="I28" s="60"/>
-      <c r="J28" s="61"/>
-      <c r="K28" s="62"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="55"/>
-      <c r="B29" s="56"/>
-      <c r="C29" s="57"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="58"/>
-      <c r="H29" s="59"/>
-      <c r="I29" s="60"/>
-      <c r="J29" s="61"/>
-      <c r="K29" s="62"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="63" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" s="64"/>
-      <c r="C30" s="65">
-        <v>0</v>
-      </c>
-      <c r="D30" s="66"/>
-      <c r="E30" s="67"/>
-      <c r="F30" s="68"/>
-      <c r="G30" s="69"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="70">
-        <v>0</v>
-      </c>
-      <c r="J30" s="71"/>
-      <c r="K30" s="72"/>
-    </row>
-    <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="73" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" s="74"/>
-      <c r="C31" s="65">
-        <v>0</v>
-      </c>
-      <c r="D31" s="66"/>
-      <c r="E31" s="67"/>
-      <c r="F31" s="69"/>
-      <c r="G31" s="69"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="70">
-        <v>0</v>
-      </c>
-      <c r="J31" s="71"/>
-      <c r="K31" s="72"/>
-    </row>
-    <row r="32" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="75" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32" s="76"/>
-      <c r="C32" s="77">
-        <v>0</v>
-      </c>
-      <c r="D32" s="78"/>
-      <c r="E32" s="79"/>
-      <c r="F32" s="68"/>
-      <c r="G32" s="69"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="70">
-        <v>0</v>
-      </c>
-      <c r="J32" s="71"/>
-      <c r="K32" s="72"/>
-    </row>
-    <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="80"/>
-      <c r="B33" s="81"/>
-      <c r="C33" s="81"/>
-      <c r="D33" s="81"/>
-      <c r="E33" s="81"/>
-      <c r="F33" s="82"/>
-      <c r="G33" s="83"/>
-      <c r="H33" s="84"/>
-      <c r="I33" s="85">
-        <v>0</v>
-      </c>
-      <c r="J33" s="86"/>
-      <c r="K33" s="87"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="88" t="s">
-        <v>27</v>
-      </c>
-      <c r="B34" s="89"/>
-      <c r="C34" s="89"/>
-      <c r="D34" s="89"/>
-      <c r="E34" s="89"/>
-      <c r="F34" s="68"/>
-      <c r="G34" s="69"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="25"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
-      <c r="J34" s="71"/>
-      <c r="K34" s="72"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="88"/>
-      <c r="B35" s="68"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="28"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="35"/>
+      <c r="B35" s="24"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="68"/>
-      <c r="G35" s="69"/>
+      <c r="F35" s="24"/>
+      <c r="G35" s="25"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
-      <c r="J35" s="71"/>
-      <c r="K35" s="72"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="88"/>
-      <c r="B36" s="68"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="28"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="35"/>
+      <c r="B36" s="24"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
-      <c r="F36" s="68"/>
-      <c r="G36" s="69"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="25"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
-      <c r="J36" s="71"/>
-      <c r="K36" s="72"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="88"/>
-      <c r="B37" s="68"/>
+      <c r="J36" s="27"/>
+      <c r="K36" s="28"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="35"/>
+      <c r="B37" s="24"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
-      <c r="F37" s="68"/>
-      <c r="G37" s="69"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="25"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
-      <c r="J37" s="71"/>
-      <c r="K37" s="72"/>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" s="88"/>
-      <c r="B38" s="68"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="28"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="35"/>
+      <c r="B38" s="24"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
-      <c r="F38" s="68"/>
-      <c r="G38" s="69"/>
+      <c r="F38" s="24"/>
+      <c r="G38" s="25"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
-      <c r="J38" s="71"/>
-      <c r="K38" s="72"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="88"/>
-      <c r="B39" s="68"/>
+      <c r="J38" s="27"/>
+      <c r="K38" s="28"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="35"/>
+      <c r="B39" s="24"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
-      <c r="F39" s="68"/>
-      <c r="G39" s="69"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="25"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
-      <c r="J39" s="71"/>
-      <c r="K39" s="72"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="88"/>
-      <c r="B40" s="68"/>
+      <c r="J39" s="27"/>
+      <c r="K39" s="28"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="35"/>
+      <c r="B40" s="24"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="68"/>
-      <c r="G40" s="69"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="25"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
-      <c r="J40" s="71"/>
-      <c r="K40" s="72"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="88"/>
-      <c r="B41" s="68"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="28"/>
+      <c r="L40" s="97"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="35"/>
+      <c r="B41" s="24"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
-      <c r="F41" s="68"/>
-      <c r="G41" s="69"/>
+      <c r="F41" s="24"/>
+      <c r="G41" s="25"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
-      <c r="J41" s="71"/>
-      <c r="K41" s="72"/>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="90"/>
-      <c r="B42" s="91"/>
-      <c r="C42" s="91"/>
-      <c r="D42" s="91"/>
+      <c r="J41" s="27"/>
+      <c r="K41" s="28"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="36"/>
+      <c r="B42" s="54"/>
+      <c r="C42" s="54"/>
+      <c r="D42" s="54"/>
       <c r="E42" s="1"/>
-      <c r="F42" s="92"/>
-      <c r="G42" s="92"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="39"/>
       <c r="H42" s="1"/>
-      <c r="I42" s="93"/>
-      <c r="J42" s="93"/>
-      <c r="K42" s="94"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="90"/>
-      <c r="B43" s="92"/>
-      <c r="C43" s="92"/>
-      <c r="D43" s="92"/>
+      <c r="I42" s="40"/>
+      <c r="J42" s="40"/>
+      <c r="K42" s="41"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="36"/>
+      <c r="B43" s="39"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="39"/>
       <c r="E43" s="1"/>
-      <c r="F43" s="92"/>
-      <c r="G43" s="92"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="39"/>
       <c r="H43" s="1"/>
-      <c r="I43" s="93"/>
-      <c r="J43" s="93"/>
-      <c r="K43" s="94"/>
-    </row>
-    <row r="44" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="95"/>
-      <c r="B44" s="84"/>
-      <c r="C44" s="84"/>
-      <c r="D44" s="84"/>
-      <c r="E44" s="84"/>
-      <c r="F44" s="84"/>
-      <c r="G44" s="84"/>
-      <c r="H44" s="84"/>
-      <c r="I44" s="96"/>
-      <c r="J44" s="84"/>
-      <c r="K44" s="87"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
+      <c r="K43" s="41"/>
+    </row>
+    <row r="44" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="37"/>
+      <c r="B44" s="31"/>
+      <c r="C44" s="31"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="31"/>
+      <c r="G44" s="31"/>
+      <c r="H44" s="31"/>
+      <c r="I44" s="38"/>
+      <c r="J44" s="31"/>
+      <c r="K44" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="I42:K42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="I43:K43"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="A33:E33"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B26:G26"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B28:G28"/>
-    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="B5:K5"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="J1:K3"/>
+    <mergeCell ref="C2:I2"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B6:K6"/>
+    <mergeCell ref="B7:K7"/>
+    <mergeCell ref="B8:K8"/>
+    <mergeCell ref="B9:K9"/>
+    <mergeCell ref="B10:K10"/>
+    <mergeCell ref="B11:K11"/>
+    <mergeCell ref="B12:K12"/>
+    <mergeCell ref="B13:K13"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:G17"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="B19:G19"/>
@@ -2389,26 +2393,25 @@
     <mergeCell ref="B22:G22"/>
     <mergeCell ref="B23:G23"/>
     <mergeCell ref="B24:G24"/>
-    <mergeCell ref="B12:K12"/>
-    <mergeCell ref="B13:K13"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B6:K6"/>
-    <mergeCell ref="B7:K7"/>
-    <mergeCell ref="B8:K8"/>
-    <mergeCell ref="B9:K9"/>
-    <mergeCell ref="B10:K10"/>
-    <mergeCell ref="B11:K11"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="C1:I1"/>
-    <mergeCell ref="J1:K3"/>
-    <mergeCell ref="C2:I2"/>
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="B5:K5"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B28:G28"/>
+    <mergeCell ref="B29:G29"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:E32"/>
+    <mergeCell ref="A33:E33"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="I42:K42"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="I43:K43"/>
+    <mergeCell ref="B42:D42"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
planilha baixando de acordo com o nome
</commit_message>
<xml_diff>
--- a/public/template/lista.xlsx
+++ b/public/template/lista.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\visumOs\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6735AB-5647-4FD3-AF85-920AF7560049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDDE7994-5D91-4461-9451-639E0FFB3F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{2C302A75-16A8-4378-A928-C1553DDDA203}"/>
+    <workbookView xWindow="-28920" yWindow="-3045" windowWidth="29040" windowHeight="15720" xr2:uid="{789B6E72-ABC1-45BD-9D34-11EE6B5E9C07}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,38 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="2">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="2">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+    <bk>
+      <rc t="1" v="1"/>
+    </bk>
+  </valueMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -113,8 +145,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="#,##0.0"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;R$&quot;* #,##0.00_);_(&quot;R$&quot;* \(#,##0.00\);_(&quot;R$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_(&quot;R$ &quot;* #,##0.00_);_(&quot;R$ &quot;* \(#,##0.00\);_(&quot;R$ &quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
@@ -667,12 +699,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -729,10 +758,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -742,6 +771,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -779,14 +811,140 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="2" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="12" fontId="2" fillId="2" borderId="18" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -794,15 +952,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -818,142 +967,20 @@
     <xf numFmtId="166" fontId="13" fillId="0" borderId="24" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="2" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="12" fontId="2" fillId="2" borderId="18" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -974,155 +1001,20 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>43624</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>176</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagem 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A992956A-EBE8-4613-91A2-BC144AED1A5C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="43624" y="200201"/>
-          <a:ext cx="689801" cy="685624"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>1979718</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>62865</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="D:\Humberto\TD\Produtos\visiumb.jpg">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9AEB5396-2325-409A-A8F7-21C4E94C9018}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="5591175" y="0"/>
-          <a:ext cx="2484543" cy="701040"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>329259</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>148601</xdr:rowOff>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2784865" cy="781240"/>
+    <xdr:ext cx="2057400" cy="1123950"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="CaixaDeTexto 3">
+        <xdr:cNvPr id="2" name="CaixaDeTexto 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED83BC0A-D56B-45A2-BEA0-F5C06367B06A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0A42A9B-0F81-4750-B590-E4EA2546CC90}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1130,8 +1022,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="329259" y="7844801"/>
-          <a:ext cx="2784865" cy="781240"/>
+          <a:off x="247650" y="7381875"/>
+          <a:ext cx="2057400" cy="1123950"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1154,7 +1046,7 @@
       </xdr:style>
       <xdr:txBody>
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="ctr">
-          <a:spAutoFit/>
+          <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
@@ -1188,18 +1080,18 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>402323</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>158126</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>131062</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2784865" cy="781240"/>
+    <xdr:ext cx="2253738" cy="953466"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="CaixaDeTexto 4">
+        <xdr:cNvPr id="3" name="CaixaDeTexto 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81A66519-88B0-49F7-A15A-F99E206BB4A0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B22FC470-C587-41EA-B01E-54671E86037F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1207,8 +1099,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4526648" y="7854326"/>
-          <a:ext cx="2784865" cy="781240"/>
+          <a:off x="2762250" y="7360537"/>
+          <a:ext cx="2253738" cy="953466"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1230,7 +1122,7 @@
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="ctr">
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr">
           <a:spAutoFit/>
         </a:bodyPr>
         <a:lstStyle/>
@@ -1265,18 +1157,18 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>551576</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>81538</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>168968</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="2309735" cy="953466"/>
+    <xdr:ext cx="1737361" cy="1125693"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="CaixaDeTexto 5">
+        <xdr:cNvPr id="4" name="CaixaDeTexto 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F363FA2-5EE8-481E-B6C7-A0994885EB59}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1AEB653-8E9D-44EC-AED7-05B3ECDDD890}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1284,8 +1176,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4818776" y="7501513"/>
-          <a:ext cx="2309735" cy="953466"/>
+          <a:off x="5391150" y="7207943"/>
+          <a:ext cx="1737361" cy="1125693"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1307,7 +1199,7 @@
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="ctr">
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr">
           <a:spAutoFit/>
         </a:bodyPr>
         <a:lstStyle/>
@@ -1400,6 +1292,81 @@
     <xdr:clientData/>
   </xdr:oneCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+  <rv s="0">
+    <v>0</v>
+    <v>5</v>
+  </rv>
+  <rv s="1">
+    <v>1</v>
+    <v>5</v>
+    <v>D:\Humberto\TD\Produtos\visiumb.jpg</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+  <s t="_localImage">
+    <k n="_rvRel:LocalImageIdentifier" t="i"/>
+    <k n="CalcOrigin" t="i"/>
+  </s>
+  <s t="_localImage">
+    <k n="_rvRel:LocalImageIdentifier" t="i"/>
+    <k n="CalcOrigin" t="i"/>
+    <k n="Text" t="s"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
+<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rel r:id="rId1"/>
+  <rel r:id="rId2"/>
+</richValueRels>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1718,448 +1685,452 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B25EF2AA-BC79-42C1-8634-CA5B31B1005A}">
-  <dimension ref="A1:L44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3577D8E-09FB-449D-9AB4-55563C65D652}">
+  <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="11" max="11" width="33.140625" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="78"/>
-      <c r="B1" s="79"/>
-      <c r="C1" s="82" t="s">
+      <c r="A1" s="42" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="84"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="47" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K1" s="48"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="80"/>
-      <c r="B2" s="81"/>
-      <c r="C2" s="89" t="s">
+      <c r="A2" s="44"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="90"/>
-      <c r="E2" s="90"/>
-      <c r="F2" s="90"/>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="86"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="50"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="88"/>
+      <c r="A3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="52"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="91">
+      <c r="B4" s="55">
         <v>5700013731</v>
       </c>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="92"/>
-      <c r="G4" s="92"/>
-      <c r="H4" s="92"/>
-      <c r="I4" s="92"/>
-      <c r="J4" s="92"/>
-      <c r="K4" s="93"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="57"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="94" t="s">
+      <c r="B5" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="95"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="95"/>
-      <c r="F5" s="95"/>
-      <c r="G5" s="95"/>
-      <c r="H5" s="95"/>
-      <c r="I5" s="95"/>
-      <c r="J5" s="95"/>
-      <c r="K5" s="96"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="41"/>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="69"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="70"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70"/>
-      <c r="J6" s="70"/>
-      <c r="K6" s="71"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="62"/>
+      <c r="F6" s="62"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="62"/>
+      <c r="J6" s="62"/>
+      <c r="K6" s="63"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="72"/>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="73"/>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73"/>
-      <c r="K7" s="74"/>
+      <c r="B7" s="64"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="66"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="60"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="61"/>
-      <c r="K8" s="62"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="68"/>
+      <c r="J8" s="68"/>
+      <c r="K8" s="69"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="69"/>
-      <c r="C9" s="70"/>
-      <c r="D9" s="70"/>
-      <c r="E9" s="70"/>
-      <c r="F9" s="70"/>
-      <c r="G9" s="70"/>
-      <c r="H9" s="70"/>
-      <c r="I9" s="70"/>
-      <c r="J9" s="70"/>
-      <c r="K9" s="71"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="62"/>
+      <c r="J9" s="62"/>
+      <c r="K9" s="63"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="75"/>
-      <c r="C10" s="76"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="76"/>
-      <c r="G10" s="76"/>
-      <c r="H10" s="76"/>
-      <c r="I10" s="76"/>
-      <c r="J10" s="76"/>
-      <c r="K10" s="77"/>
+      <c r="B10" s="70"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="71"/>
+      <c r="H10" s="71"/>
+      <c r="I10" s="71"/>
+      <c r="J10" s="71"/>
+      <c r="K10" s="72"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="60"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="61"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="61"/>
-      <c r="K11" s="62"/>
+      <c r="B11" s="67"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="68"/>
+      <c r="I11" s="68"/>
+      <c r="J11" s="68"/>
+      <c r="K11" s="69"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="60"/>
-      <c r="C12" s="61"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="61"/>
-      <c r="H12" s="61"/>
-      <c r="I12" s="61"/>
-      <c r="J12" s="61"/>
-      <c r="K12" s="62"/>
+      <c r="B12" s="67"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="68"/>
+      <c r="E12" s="68"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="68"/>
+      <c r="I12" s="68"/>
+      <c r="J12" s="68"/>
+      <c r="K12" s="69"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="63"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="64"/>
-      <c r="I13" s="64"/>
-      <c r="J13" s="64"/>
-      <c r="K13" s="65"/>
+      <c r="B13" s="73"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="74"/>
+      <c r="H13" s="74"/>
+      <c r="I13" s="74"/>
+      <c r="J13" s="74"/>
+      <c r="K13" s="75"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="14"/>
+      <c r="A14" s="8"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="13"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="66" t="s">
+      <c r="B15" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="67"/>
-      <c r="D15" s="67"/>
-      <c r="E15" s="67"/>
-      <c r="F15" s="67"/>
-      <c r="G15" s="68"/>
-      <c r="H15" s="16" t="s">
+      <c r="C15" s="77"/>
+      <c r="D15" s="77"/>
+      <c r="E15" s="77"/>
+      <c r="F15" s="77"/>
+      <c r="G15" s="78"/>
+      <c r="H15" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="17" t="s">
+      <c r="I15" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="J15" s="16" t="s">
+      <c r="J15" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="K15" s="18" t="s">
+      <c r="K15" s="17" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
-      <c r="B16" s="55"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="57"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="23"/>
+      <c r="A16" s="18"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="22"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
-      <c r="B17" s="55"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="57"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="23"/>
+      <c r="A17" s="18"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="59"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="22"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
-      <c r="B18" s="55"/>
-      <c r="C18" s="56"/>
-      <c r="D18" s="56"/>
-      <c r="E18" s="56"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="57"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="23"/>
+      <c r="A18" s="18"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="22"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
-      <c r="B19" s="55"/>
-      <c r="C19" s="56"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="56"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="23"/>
+      <c r="A19" s="18"/>
+      <c r="B19" s="58"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="60"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="22"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
-      <c r="B20" s="55"/>
-      <c r="C20" s="56"/>
-      <c r="D20" s="56"/>
-      <c r="E20" s="56"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="57"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="23"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="58"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="60"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="22"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
-      <c r="B21" s="55"/>
-      <c r="C21" s="56"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="56"/>
-      <c r="F21" s="56"/>
-      <c r="G21" s="57"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="23"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="58"/>
+      <c r="C21" s="59"/>
+      <c r="D21" s="59"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="60"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="22"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
-      <c r="B22" s="55"/>
-      <c r="C22" s="56"/>
-      <c r="D22" s="56"/>
-      <c r="E22" s="56"/>
-      <c r="F22" s="56"/>
-      <c r="G22" s="57"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="23"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="22"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
-      <c r="B23" s="55"/>
-      <c r="C23" s="56"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="56"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="57"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="21"/>
-      <c r="J23" s="22"/>
-      <c r="K23" s="23"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="58"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="22"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
-      <c r="B24" s="55"/>
-      <c r="C24" s="56"/>
-      <c r="D24" s="56"/>
-      <c r="E24" s="56"/>
-      <c r="F24" s="56"/>
-      <c r="G24" s="57"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="23"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="58"/>
+      <c r="C24" s="59"/>
+      <c r="D24" s="59"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="60"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="22"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="19"/>
-      <c r="B25" s="55"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="56"/>
-      <c r="E25" s="56"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="57"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="23"/>
+      <c r="A25" s="18"/>
+      <c r="B25" s="58"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="60"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="22"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="19"/>
-      <c r="B26" s="55"/>
-      <c r="C26" s="56"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="56"/>
-      <c r="F26" s="56"/>
-      <c r="G26" s="57"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="21"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="23"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="58"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="60"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="22"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="19"/>
-      <c r="B27" s="55"/>
-      <c r="C27" s="56"/>
-      <c r="D27" s="56"/>
-      <c r="E27" s="56"/>
-      <c r="F27" s="56"/>
-      <c r="G27" s="57"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="21"/>
-      <c r="J27" s="22"/>
-      <c r="K27" s="23"/>
+      <c r="A27" s="18"/>
+      <c r="B27" s="58"/>
+      <c r="C27" s="59"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="22"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="19"/>
-      <c r="B28" s="55"/>
-      <c r="C28" s="56"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="56"/>
-      <c r="F28" s="56"/>
-      <c r="G28" s="57"/>
-      <c r="H28" s="20"/>
-      <c r="I28" s="21"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="23"/>
+      <c r="A28" s="18"/>
+      <c r="B28" s="58"/>
+      <c r="C28" s="59"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="59"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="60"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="22"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="19"/>
-      <c r="B29" s="55"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="56"/>
-      <c r="F29" s="56"/>
-      <c r="G29" s="57"/>
-      <c r="H29" s="20"/>
-      <c r="I29" s="21"/>
-      <c r="J29" s="22"/>
-      <c r="K29" s="23"/>
+      <c r="A29" s="18"/>
+      <c r="B29" s="58"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="59"/>
+      <c r="F29" s="59"/>
+      <c r="G29" s="60"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="22"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="58" t="s">
+      <c r="A30" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="59"/>
-      <c r="C30" s="44">
+      <c r="B30" s="80"/>
+      <c r="C30" s="81">
         <v>0</v>
       </c>
-      <c r="D30" s="45"/>
-      <c r="E30" s="46"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="1"/>
+      <c r="D30" s="82"/>
+      <c r="E30" s="83"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="25"/>
       <c r="I30" s="26">
         <v>0</v>
       </c>
@@ -2167,18 +2138,18 @@
       <c r="K30" s="28"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="42" t="s">
+      <c r="A31" s="84" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="43"/>
-      <c r="C31" s="44">
+      <c r="B31" s="85"/>
+      <c r="C31" s="81">
         <v>0</v>
       </c>
-      <c r="D31" s="45"/>
-      <c r="E31" s="46"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="1"/>
+      <c r="D31" s="82"/>
+      <c r="E31" s="83"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="25"/>
       <c r="I31" s="26">
         <v>0</v>
       </c>
@@ -2186,30 +2157,30 @@
       <c r="K31" s="28"/>
     </row>
     <row r="32" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="47" t="s">
+      <c r="A32" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="B32" s="48"/>
-      <c r="C32" s="49">
+      <c r="B32" s="87"/>
+      <c r="C32" s="88">
         <v>0</v>
       </c>
-      <c r="D32" s="50"/>
-      <c r="E32" s="51"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="1"/>
+      <c r="D32" s="89"/>
+      <c r="E32" s="90"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="25"/>
       <c r="I32" s="26">
         <v>0</v>
       </c>
       <c r="J32" s="27"/>
       <c r="K32" s="28"/>
     </row>
-    <row r="33" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="52"/>
-      <c r="B33" s="53"/>
-      <c r="C33" s="53"/>
-      <c r="D33" s="53"/>
-      <c r="E33" s="53"/>
+    <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="95"/>
+      <c r="B33" s="96"/>
+      <c r="C33" s="96"/>
+      <c r="D33" s="96"/>
+      <c r="E33" s="96"/>
       <c r="F33" s="29"/>
       <c r="G33" s="30"/>
       <c r="H33" s="31"/>
@@ -2219,140 +2190,139 @@
       <c r="J33" s="33"/>
       <c r="K33" s="34"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="25"/>
       <c r="J34" s="27"/>
       <c r="K34" s="28"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="35"/>
-      <c r="B35" s="24"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="24"/>
+      <c r="H35" s="25"/>
+      <c r="I35" s="25"/>
       <c r="J35" s="27"/>
       <c r="K35" s="28"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="35"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="25"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="25"/>
+      <c r="I36" s="25"/>
       <c r="J36" s="27"/>
       <c r="K36" s="28"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="35"/>
-      <c r="B37" s="24"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="24"/>
+      <c r="H37" s="25"/>
+      <c r="I37" s="25"/>
       <c r="J37" s="27"/>
       <c r="K37" s="28"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="35"/>
-      <c r="B38" s="24"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="24"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="25"/>
       <c r="J38" s="27"/>
       <c r="K38" s="28"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="35"/>
-      <c r="B39" s="24"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="25"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="24"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="25"/>
       <c r="J39" s="27"/>
       <c r="K39" s="28"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="35"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="25"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="24"/>
+      <c r="H40" s="25"/>
+      <c r="I40" s="25"/>
       <c r="J40" s="27"/>
       <c r="K40" s="28"/>
-      <c r="L40" s="97"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="35"/>
-      <c r="B41" s="24"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="24"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="24"/>
+      <c r="H41" s="25"/>
+      <c r="I41" s="25"/>
       <c r="J41" s="27"/>
       <c r="K41" s="28"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="36"/>
-      <c r="B42" s="54"/>
-      <c r="C42" s="54"/>
-      <c r="D42" s="54"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="39"/>
-      <c r="H42" s="1"/>
-      <c r="I42" s="40"/>
-      <c r="J42" s="40"/>
-      <c r="K42" s="41"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B42" s="94"/>
+      <c r="C42" s="94"/>
+      <c r="D42" s="94"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="91"/>
+      <c r="G42" s="91"/>
+      <c r="H42" s="25"/>
+      <c r="I42" s="92"/>
+      <c r="J42" s="92"/>
+      <c r="K42" s="93"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="36"/>
-      <c r="B43" s="39"/>
-      <c r="C43" s="39"/>
-      <c r="D43" s="39"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="39"/>
-      <c r="G43" s="39"/>
-      <c r="H43" s="1"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
-      <c r="K43" s="41"/>
-    </row>
-    <row r="44" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="91"/>
+      <c r="C43" s="91"/>
+      <c r="D43" s="91"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="91"/>
+      <c r="G43" s="91"/>
+      <c r="H43" s="25"/>
+      <c r="I43" s="92"/>
+      <c r="J43" s="92"/>
+      <c r="K43" s="93"/>
+    </row>
+    <row r="44" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="37"/>
       <c r="B44" s="31"/>
       <c r="C44" s="31"/>
@@ -2366,25 +2336,11 @@
       <c r="K44" s="34"/>
     </row>
   </sheetData>
-  <mergeCells count="42">
-    <mergeCell ref="B5:K5"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="C1:I1"/>
-    <mergeCell ref="J1:K3"/>
-    <mergeCell ref="C2:I2"/>
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B6:K6"/>
-    <mergeCell ref="B7:K7"/>
-    <mergeCell ref="B8:K8"/>
-    <mergeCell ref="B9:K9"/>
-    <mergeCell ref="B10:K10"/>
-    <mergeCell ref="B11:K11"/>
-    <mergeCell ref="B12:K12"/>
-    <mergeCell ref="B13:K13"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B17:G17"/>
+  <mergeCells count="35">
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:E32"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="B19:G19"/>
@@ -2398,20 +2354,26 @@
     <mergeCell ref="B27:G27"/>
     <mergeCell ref="B28:G28"/>
     <mergeCell ref="B29:G29"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:E32"/>
-    <mergeCell ref="A33:E33"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="I42:K42"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="I43:K43"/>
-    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B6:K6"/>
+    <mergeCell ref="B7:K7"/>
+    <mergeCell ref="B8:K8"/>
+    <mergeCell ref="B9:K9"/>
+    <mergeCell ref="B10:K10"/>
+    <mergeCell ref="B11:K11"/>
+    <mergeCell ref="B12:K12"/>
+    <mergeCell ref="B13:K13"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B5:K5"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="J1:K3"/>
+    <mergeCell ref="C2:I2"/>
+    <mergeCell ref="B4:K4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>